<commit_message>
Added borders to the table.
</commit_message>
<xml_diff>
--- a/Week4_LineOfBalance.xlsx
+++ b/Week4_LineOfBalance.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="12120" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="12120" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet1!$A$1:$K$16</definedName>
+  </definedNames>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Activity</t>
   </si>
@@ -110,15 +113,18 @@
   <si>
     <t>End First Unit</t>
   </si>
+  <si>
+    <t>WEEK 4: Line of Balance Diagram</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -149,6 +155,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -158,12 +181,51 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -222,12 +284,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -290,12 +372,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -355,7 +440,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -392,10 +476,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0562962956134548"/>
-          <c:y val="0.125418702256809"/>
-          <c:w val="0.911190547769946"/>
-          <c:h val="0.794433087328079"/>
+          <c:x val="5.6296295613454797E-2"/>
+          <c:y val="0.12541870225680901"/>
+          <c:w val="0.91119054776994601"/>
+          <c:h val="0.79443308732807905"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -460,7 +544,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -481,12 +564,12 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$M$8:$P$8</c:f>
+              <c:f>Sheet1!$M$10:$P$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>29.6875</c:v>
@@ -502,26 +585,31 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$17:$B$20</c:f>
+              <c:f>Sheet1!$B$19:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-29AD-7B49-8A7F-6362EC19690A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -582,7 +670,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -603,7 +690,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$M$9:$P$9</c:f>
+              <c:f>Sheet1!$M$11:$P$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -611,39 +698,44 @@
                   <c:v>8.125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42.76041666666666</c:v>
+                  <c:v>42.760416666666664</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.05208333333333</c:v>
+                  <c:v>50.052083333333329</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.41666666666666</c:v>
+                  <c:v>15.416666666666664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$17:$B$20</c:f>
+              <c:f>Sheet1!$B$19:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-29AD-7B49-8A7F-6362EC19690A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -704,7 +796,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -725,47 +816,52 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$M$10:$P$10</c:f>
+              <c:f>Sheet1!$M$12:$P$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>20.41666666666666</c:v>
+                  <c:v>20.416666666666664</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>56.04166666666666</c:v>
+                  <c:v>56.041666666666664</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>59.79166666666666</c:v>
+                  <c:v>59.791666666666664</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.16666666666666</c:v>
+                  <c:v>24.166666666666664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$17:$B$20</c:f>
+              <c:f>Sheet1!$B$19:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-29AD-7B49-8A7F-6362EC19690A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -826,7 +922,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -847,47 +942,52 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$M$11:$P$11</c:f>
+              <c:f>Sheet1!$M$13:$P$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>33.12499999999998</c:v>
+                  <c:v>33.124999999999986</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64.79166666666665</c:v>
+                  <c:v>64.791666666666657</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>69.79166666666665</c:v>
+                  <c:v>69.791666666666657</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38.12499999999998</c:v>
+                  <c:v>38.124999999999986</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$17:$B$20</c:f>
+              <c:f>Sheet1!$B$19:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-29AD-7B49-8A7F-6362EC19690A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -912,8 +1012,8 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.00695098932018395"/>
-                  <c:y val="-0.0353240119374951"/>
+                  <c:x val="-6.95098932018395E-3"/>
+                  <c:y val="-3.5324011937495098E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -924,8 +1024,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-29AD-7B49-8A7F-6362EC19690A}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -933,8 +1034,8 @@
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.0354814686184546"/>
-                  <c:y val="-0.0514634900700113"/>
+                  <c:x val="3.5481468618454602E-2"/>
+                  <c:y val="-5.1463490070011303E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -945,8 +1046,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-29AD-7B49-8A7F-6362EC19690A}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -990,7 +1092,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1011,47 +1112,52 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$M$12:$P$12</c:f>
+              <c:f>Sheet1!$M$14:$P$14</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>52.52604166666666</c:v>
+                  <c:v>52.526041666666657</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>74.79166666666665</c:v>
+                  <c:v>74.791666666666657</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>77.13541666666666</c:v>
+                  <c:v>77.135416666666657</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>54.86979166666666</c:v>
+                  <c:v>54.869791666666657</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$17:$B$20</c:f>
+              <c:f>Sheet1!$B$19:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-29AD-7B49-8A7F-6362EC19690A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1068,7 +1174,7 @@
         <c:axId val="-1326733024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="80.0"/>
+          <c:max val="80"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1107,7 +1213,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1182,7 +1287,7 @@
         <c:axId val="-1326727872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="20.0"/>
+          <c:max val="20"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1221,7 +1326,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1251,6 +1355,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1307,9 +1412,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0672668356929839"/>
-          <c:y val="0.331839266683113"/>
-          <c:w val="0.0797578290669418"/>
+          <c:x val="6.7266835692983903E-2"/>
+          <c:y val="0.33183926668311298"/>
+          <c:w val="7.9757829066941802E-2"/>
           <c:h val="0.190633984404077"/>
         </c:manualLayout>
       </c:layout>
@@ -1932,10 +2037,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" workbookViewId="0"/>
+    <sheetView zoomScale="162" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -1950,7 +2055,13 @@
     <xdr:ext cx="8678333" cy="6295123"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks noGrp="1"/>
         </xdr:cNvGraphicFramePr>
@@ -2473,454 +2584,475 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="110" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="108" zoomScaleNormal="110" zoomScaleSheetLayoutView="108" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.6640625" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" customWidth="1"/>
+    <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2">
-        <v>20</v>
+      <c r="A1" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
         <v>8</v>
       </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
+      <c r="C5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>1</v>
+      <c r="A6" t="s">
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
         <v>5</v>
       </c>
-      <c r="F6">
-        <v>6</v>
-      </c>
-      <c r="G6">
-        <v>7</v>
-      </c>
-      <c r="H6">
-        <v>8</v>
-      </c>
-      <c r="I6">
+      <c r="C6" t="s">
         <v>9</v>
-      </c>
-      <c r="M6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N6" t="s">
-        <v>24</v>
-      </c>
-      <c r="O6" t="s">
-        <v>25</v>
-      </c>
-      <c r="P6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" t="s">
-        <v>5</v>
-      </c>
-      <c r="K7" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="16">
+        <v>1</v>
+      </c>
+      <c r="B8" s="16">
+        <v>2</v>
+      </c>
+      <c r="C8" s="16">
+        <v>3</v>
+      </c>
+      <c r="D8" s="16">
+        <v>4</v>
+      </c>
+      <c r="E8" s="16">
+        <v>5</v>
+      </c>
+      <c r="F8" s="16">
+        <v>6</v>
+      </c>
+      <c r="G8" s="16">
+        <v>7</v>
+      </c>
+      <c r="H8" s="16">
+        <v>8</v>
+      </c>
+      <c r="I8" s="16">
+        <v>9</v>
+      </c>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="M8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8" t="s">
+        <v>25</v>
+      </c>
+      <c r="P8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" s="4" customFormat="1" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B10" s="6">
         <v>100</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C10" s="6">
         <v>4</v>
       </c>
-      <c r="D8" s="2">
-        <f>B8*$B$1/($B$3*$B$4)</f>
+      <c r="D10" s="7">
+        <f>B10*$B$3/($B$5*$B$6)</f>
         <v>7.5</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E10" s="6">
         <v>8</v>
       </c>
-      <c r="F8" s="1">
-        <f>E8/D8*$B$1</f>
+      <c r="F10" s="8">
+        <f>E10/D10*$B$3</f>
         <v>3.2</v>
       </c>
-      <c r="G8" s="1">
-        <f>B8/(C8*$B$3)</f>
+      <c r="G10" s="8">
+        <f>B10/(C10*$B$5)</f>
         <v>3.125</v>
       </c>
-      <c r="H8" s="1">
-        <f>($B$2-1)*$B$4/F8</f>
+      <c r="H10" s="8">
+        <f>($B$4-1)*$B$6/F10</f>
         <v>29.6875</v>
       </c>
-      <c r="I8">
+      <c r="I10" s="9">
         <v>5</v>
       </c>
-      <c r="K8" t="str">
-        <f>IF(F8&gt;F9,"After 1st unit", "After last unit")</f>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9" t="str">
+        <f>IF(F10&gt;F11,"After 1st unit", "After last unit")</f>
         <v>After 1st unit</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M10" s="1">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="N8" s="1">
-        <f t="shared" ref="N8:N13" si="0">M8+H8</f>
+      <c r="N10" s="1">
+        <f t="shared" ref="N10:N15" si="0">M10+H10</f>
         <v>29.6875</v>
       </c>
-      <c r="O8" s="1">
-        <f t="shared" ref="O8:O13" si="1">N8+G8</f>
+      <c r="O10" s="1">
+        <f t="shared" ref="O10:O15" si="1">N10+G10</f>
         <v>32.8125</v>
       </c>
-      <c r="P8" s="1">
-        <f t="shared" ref="P8:P13" si="2">O8-N8+M8</f>
+      <c r="P10" s="1">
+        <f t="shared" ref="P10:P15" si="2">O10-N10+M10</f>
         <v>3.125</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B11" s="6">
         <v>350</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C11" s="6">
         <v>6</v>
       </c>
-      <c r="D9" s="2">
-        <f>B9*$B$1/($B$3*$B$4)</f>
+      <c r="D11" s="7">
+        <f>B11*$B$3/($B$5*$B$6)</f>
         <v>26.25</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E11" s="6">
         <v>24</v>
       </c>
-      <c r="F9" s="1">
-        <f>E9/D9*$B$1</f>
+      <c r="F11" s="8">
+        <f>E11/D11*$B$3</f>
         <v>2.7428571428571429</v>
       </c>
-      <c r="G9" s="1">
-        <f>B9/(C9*$B$3)</f>
+      <c r="G11" s="8">
+        <f>B11/(C11*$B$5)</f>
         <v>7.291666666666667</v>
       </c>
-      <c r="H9" s="1">
-        <f>($B$2-1)*$B$4/F9</f>
+      <c r="H11" s="8">
+        <f>($B$4-1)*$B$6/F11</f>
         <v>34.635416666666664</v>
       </c>
-      <c r="I9">
+      <c r="I11" s="9">
         <v>5</v>
       </c>
-      <c r="K9" t="str">
-        <f>IF(F9&gt;F10,"After 1st unit", "After last unit")</f>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9" t="str">
+        <f>IF(F11&gt;F12,"After 1st unit", "After last unit")</f>
         <v>After 1st unit</v>
       </c>
-      <c r="M9" s="1">
-        <f>IF(K8="After 1st unit",P8+I8,O8+I8-H9)</f>
+      <c r="M11" s="1">
+        <f>IF(K10="After 1st unit",P10+I10,O10+I10-H11)</f>
         <v>8.125</v>
       </c>
-      <c r="N9" s="1">
+      <c r="N11" s="1">
         <f t="shared" si="0"/>
         <v>42.760416666666664</v>
       </c>
-      <c r="O9" s="1">
+      <c r="O11" s="1">
         <f t="shared" si="1"/>
         <v>50.052083333333329</v>
       </c>
-      <c r="P9" s="1">
+      <c r="P11" s="1">
         <f t="shared" si="2"/>
         <v>15.416666666666664</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B12" s="6">
         <v>60</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C12" s="6">
         <v>2</v>
       </c>
-      <c r="D10" s="2">
-        <f>B10*$B$1/($B$3*$B$4)</f>
+      <c r="D12" s="7">
+        <f>B12*$B$3/($B$5*$B$6)</f>
         <v>4.5</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E12" s="6">
         <v>4</v>
       </c>
-      <c r="F10" s="1">
-        <f>E10/D10*$B$1</f>
+      <c r="F12" s="8">
+        <f>E12/D12*$B$3</f>
         <v>2.6666666666666665</v>
       </c>
-      <c r="G10" s="1">
-        <f>B10/(C10*$B$3)</f>
+      <c r="G12" s="8">
+        <f>B12/(C12*$B$5)</f>
         <v>3.75</v>
       </c>
-      <c r="H10" s="1">
-        <f>($B$2-1)*$B$4/F10</f>
+      <c r="H12" s="8">
+        <f>($B$4-1)*$B$6/F12</f>
         <v>35.625</v>
       </c>
-      <c r="I10">
+      <c r="I12" s="9">
         <v>5</v>
       </c>
-      <c r="K10" t="str">
-        <f>IF(F10&gt;F11,"After 1st unit", "After last unit")</f>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9" t="str">
+        <f>IF(F12&gt;F13,"After 1st unit", "After last unit")</f>
         <v>After last unit</v>
       </c>
-      <c r="M10" s="1">
-        <f>IF(K9="After 1st unit",P9+I9,O9+I9-H10)</f>
+      <c r="M12" s="1">
+        <f>IF(K11="After 1st unit",P11+I11,O11+I11-H12)</f>
         <v>20.416666666666664</v>
       </c>
-      <c r="N10" s="1">
+      <c r="N12" s="1">
         <f t="shared" si="0"/>
         <v>56.041666666666664</v>
       </c>
-      <c r="O10" s="1">
+      <c r="O12" s="1">
         <f t="shared" si="1"/>
         <v>59.791666666666664</v>
       </c>
-      <c r="P10" s="1">
+      <c r="P12" s="1">
         <f t="shared" si="2"/>
         <v>24.166666666666664</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B13" s="6">
         <v>200</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C13" s="6">
         <v>5</v>
       </c>
-      <c r="D11" s="2">
-        <f>B11*$B$1/($B$3*$B$4)</f>
+      <c r="D13" s="7">
+        <f>B13*$B$3/($B$5*$B$6)</f>
         <v>15</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E13" s="6">
         <v>15</v>
       </c>
-      <c r="F11" s="1">
-        <f>E11/D11*$B$1</f>
+      <c r="F13" s="8">
+        <f>E13/D13*$B$3</f>
         <v>3</v>
       </c>
-      <c r="G11" s="1">
-        <f>B11/(C11*$B$3)</f>
+      <c r="G13" s="8">
+        <f>B13/(C13*$B$5)</f>
         <v>5</v>
       </c>
-      <c r="H11" s="1">
-        <f>($B$2-1)*$B$4/F11</f>
+      <c r="H13" s="8">
+        <f>($B$4-1)*$B$6/F13</f>
         <v>31.666666666666668</v>
       </c>
-      <c r="I11">
+      <c r="I13" s="9">
         <v>5</v>
       </c>
-      <c r="K11" t="str">
-        <f>IF(F11&gt;F12,"After 1st unit", "After last unit")</f>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9" t="str">
+        <f>IF(F13&gt;F14,"After 1st unit", "After last unit")</f>
         <v>After last unit</v>
       </c>
-      <c r="M11" s="1">
-        <f>IF(K10="After 1st unit",P10+I10,O10+I10-H11)</f>
+      <c r="M13" s="1">
+        <f>IF(K12="After 1st unit",P12+I12,O12+I12-H13)</f>
         <v>33.124999999999986</v>
       </c>
-      <c r="N11" s="1">
+      <c r="N13" s="1">
         <f t="shared" si="0"/>
         <v>64.791666666666657</v>
       </c>
-      <c r="O11" s="1">
+      <c r="O13" s="1">
         <f t="shared" si="1"/>
         <v>69.791666666666657</v>
       </c>
-      <c r="P11" s="1">
+      <c r="P13" s="1">
         <f t="shared" si="2"/>
         <v>38.124999999999986</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B14" s="11">
         <v>150</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C14" s="11">
         <v>8</v>
       </c>
-      <c r="D12" s="2">
-        <f>B12*$B$1/($B$3*$B$4)</f>
+      <c r="D14" s="12">
+        <f>B14*$B$3/($B$5*$B$6)</f>
         <v>11.25</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E14" s="11">
         <v>16</v>
       </c>
-      <c r="F12" s="1">
-        <f>E12/D12*$B$1</f>
+      <c r="F14" s="13">
+        <f>E14/D14*$B$3</f>
         <v>4.2666666666666666</v>
       </c>
-      <c r="G12" s="1">
-        <f>B12/(C12*$B$3)</f>
+      <c r="G14" s="13">
+        <f>B14/(C14*$B$5)</f>
         <v>2.34375</v>
       </c>
-      <c r="H12" s="1">
-        <f>($B$2-1)*$B$4/F12</f>
+      <c r="H14" s="13">
+        <f>($B$4-1)*$B$6/F14</f>
         <v>22.265625</v>
       </c>
-      <c r="I12">
+      <c r="I14" s="14">
         <v>5</v>
       </c>
-      <c r="M12" s="1">
-        <f>IF(K11="After 1st unit",P11+I11,O11+I11-H12)</f>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="M14" s="1">
+        <f>IF(K13="After 1st unit",P13+I13,O13+I13-H14)</f>
         <v>52.526041666666657</v>
       </c>
-      <c r="N12" s="1">
+      <c r="N14" s="1">
         <f t="shared" si="0"/>
         <v>74.791666666666657</v>
       </c>
-      <c r="O12" s="1">
+      <c r="O14" s="1">
         <f t="shared" si="1"/>
         <v>77.135416666666657</v>
       </c>
-      <c r="P12" s="1">
+      <c r="P14" s="1">
         <f t="shared" si="2"/>
         <v>54.869791666666657</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="M13" s="1">
-        <f>IF(K12="After 1st unit",P12+I12,O12+I12-H13)</f>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M15" s="1">
+        <f>IF(K14="After 1st unit",P14+I14,O14+I14-H15)</f>
         <v>82.135416666666657</v>
       </c>
-      <c r="N13" s="1">
+      <c r="N15" s="1">
         <f t="shared" si="0"/>
         <v>82.135416666666657</v>
       </c>
-      <c r="O13" s="1">
+      <c r="O15" s="1">
         <f t="shared" si="1"/>
         <v>82.135416666666657</v>
       </c>
-      <c r="P13" s="1">
+      <c r="P15" s="1">
         <f t="shared" si="2"/>
         <v>82.135416666666657</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="1">
-        <f>G8+I8+G9+I9+G10+H10+I10+G11+I11+G12</f>
+      <c r="B16" s="1">
+        <f>G10+I10+G11+I11+G12+H12+I12+G13+I13+G14</f>
         <v>77.135416666666671</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18">
-        <v>20</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="14:14" x14ac:dyDescent="0.2">
-      <c r="N35" s="4"/>
-    </row>
-    <row r="36" spans="14:14" x14ac:dyDescent="0.2">
-      <c r="N36" s="4"/>
     </row>
     <row r="37" spans="14:14" x14ac:dyDescent="0.2">
-      <c r="N37" s="4"/>
+      <c r="N37" s="2"/>
     </row>
     <row r="38" spans="14:14" x14ac:dyDescent="0.2">
-      <c r="N38" s="4"/>
+      <c r="N38" s="2"/>
+    </row>
+    <row r="39" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N39" s="2"/>
+    </row>
+    <row r="40" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N40" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="93" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="11" max="1048575" man="1"/>
+  </colBreaks>
 </worksheet>
 </file>
</xml_diff>